<commit_message>
fix: cambio de archivo GenItem
</commit_message>
<xml_diff>
--- a/src/assets/ejemplos/modelo/ConActivo.xlsx
+++ b/src/assets/ejemplos/modelo/ConActivo.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fecha compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha activacion</t>
   </si>
   <si>
     <t xml:space="preserve">Fecha baja</t>
@@ -140,8 +143,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -235,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,6 +253,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,7 +512,7 @@
   <dimension ref="A1:AJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,7 +523,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.11"/>
@@ -549,31 +557,31 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -601,13 +609,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>2025</v>
@@ -628,19 +636,19 @@
       <c r="K2" s="1" t="n">
         <v>200000</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="L2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="N2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="O2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P2" s="1" t="n">
+      <c r="P2" s="4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>